<commit_message>
Sweden Testdata Changes Osprey
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreySweden.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreySweden.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4B3FAD-0B82-46FF-A4F9-9066E4D0E105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{ED4B3FAD-0B82-46FF-A4F9-9066E4D0E105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0876EFBA-F1FE-4E0A-AEC2-3CD12430C2DF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="268">
   <si>
     <t>DataSet</t>
   </si>
@@ -884,6 +884,12 @@
   <si>
     <t>Succulent Green</t>
   </si>
+  <si>
+    <t>RADIAL 34</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
 </sst>
 </file>
 
@@ -892,7 +898,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1323,11 +1329,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -1339,7 +1345,7 @@
     <col min="8" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1412,67 +1418,67 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="8"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="18" spans="4:9">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="21" spans="4:9">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="4:9">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" s="9"/>
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="26" spans="4:9">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="4:9">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
@@ -1493,12 +1499,12 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1536,7 +1542,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>159</v>
       </c>
@@ -1554,27 +1560,27 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="H4" s="9"/>
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H5" s="10"/>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H6" s="5"/>
     </row>
   </sheetData>
@@ -1591,9 +1597,9 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1750,10 +1756,10 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -1761,7 +1767,7 @@
     <col min="15" max="16" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1873,7 +1879,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1890,24 +1896,24 @@
         <v>94</v>
       </c>
       <c r="S3" t="s">
-        <v>150</v>
+        <v>266</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
       <c r="N4" t="s">
-        <v>150</v>
+        <v>266</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -1918,7 +1924,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>151</v>
       </c>
@@ -1942,7 +1948,7 @@
       <selection activeCell="J2" sqref="J2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
@@ -1954,7 +1960,7 @@
     <col min="27" max="27" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>178</v>
       </c>
@@ -2170,13 +2176,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2205,7 +2211,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -2258,13 +2264,13 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2277,7 +2283,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="375">
+    <row r="2" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2309,7 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -2320,7 +2326,7 @@
     <col min="14" max="14" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2388,7 +2394,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2426,7 +2432,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2452,7 +2458,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -2472,7 +2478,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -2498,7 +2504,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="90">
+    <row r="6" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>194</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N7" s="13"/>
     </row>
   </sheetData>
@@ -2548,7 +2554,7 @@
       <selection activeCell="I2" sqref="I2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
@@ -2556,7 +2562,7 @@
     <col min="15" max="15" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2627,7 +2633,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>198</v>
       </c>
@@ -2698,7 +2704,7 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -2712,7 +2718,7 @@
     <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2776,7 +2782,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2814,7 +2820,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14.25" customHeight="1">
+    <row r="3" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -2843,7 +2849,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>204</v>
       </c>
@@ -2868,7 +2874,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -2906,7 +2912,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -2916,7 +2922,7 @@
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -3003,7 +3009,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>209</v>
       </c>
@@ -3035,7 +3041,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="56.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -3058,7 +3064,7 @@
     <col min="22" max="22" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3108,7 +3114,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3127,7 +3133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3138,7 +3144,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3149,7 +3155,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3160,7 +3166,7 @@
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -3171,7 +3177,7 @@
       <c r="P6" s="4"/>
       <c r="V6" s="5"/>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -3182,7 +3188,7 @@
       <c r="P7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3192,54 +3198,54 @@
       <c r="I8" s="2"/>
       <c r="V8" s="5"/>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="V9" s="5"/>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="V10" s="5"/>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="V11" s="5"/>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D12" s="8"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="AD12" s="10"/>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="V13" s="5"/>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="R15" s="5"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="R16" s="5"/>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="4:29">
+    <row r="17" spans="4:29" x14ac:dyDescent="0.25">
       <c r="R17" s="5"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="4:29">
+    <row r="18" spans="4:29" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="O18" s="5"/>
@@ -3249,21 +3255,21 @@
       <c r="S18" s="7"/>
       <c r="AC18" s="5"/>
     </row>
-    <row r="19" spans="4:29">
+    <row r="19" spans="4:29" x14ac:dyDescent="0.25">
       <c r="R19" s="5"/>
       <c r="S19" s="7"/>
       <c r="T19" s="5"/>
     </row>
-    <row r="20" spans="4:29">
+    <row r="20" spans="4:29" x14ac:dyDescent="0.25">
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="4:29">
+    <row r="21" spans="4:29" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="4:29">
+    <row r="22" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D22" s="9"/>
       <c r="E22" s="2"/>
       <c r="H22" s="2"/>
@@ -3271,17 +3277,17 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="4:29">
+    <row r="23" spans="4:29" x14ac:dyDescent="0.25">
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="26" spans="4:29">
+    <row r="26" spans="4:29" x14ac:dyDescent="0.25">
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="4:29">
+    <row r="27" spans="4:29" x14ac:dyDescent="0.25">
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
@@ -3295,11 +3301,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEDE721-2994-4A91-8C89-FADAE76105D8}">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -3316,7 +3322,7 @@
     <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -3448,7 +3454,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -3471,15 +3477,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
       <c r="W4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>216</v>
       </c>
@@ -3507,7 +3513,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -3521,7 +3527,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -3559,7 +3565,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>220</v>
       </c>
@@ -3590,7 +3596,7 @@
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>221</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>224</v>
       </c>
@@ -3619,7 +3625,7 @@
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>227</v>
       </c>
@@ -3640,7 +3646,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -3666,7 +3672,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>229</v>
       </c>
@@ -3712,7 +3718,7 @@
       <c r="V15" s="5"/>
       <c r="W15" s="7"/>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>235</v>
       </c>
@@ -3756,19 +3762,19 @@
       </c>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>149</v>
       </c>
       <c r="R17" t="s">
-        <v>150</v>
+        <v>266</v>
       </c>
       <c r="T17" s="5"/>
       <c r="V17" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>241</v>
       </c>
@@ -3776,7 +3782,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>242</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -3801,7 +3807,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>151</v>
       </c>
@@ -3812,7 +3818,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>245</v>
       </c>
@@ -3826,7 +3832,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>248</v>
       </c>
@@ -3866,9 +3872,9 @@
       <selection activeCell="Q12" sqref="Q12:U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3981,7 +3987,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4028,7 +4034,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>254</v>
       </c>
@@ -4054,7 +4060,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -4062,7 +4068,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -4076,7 +4082,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>216</v>
       </c>
@@ -4090,7 +4096,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -4104,7 +4110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -4118,7 +4124,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -4146,7 +4152,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -4161,7 +4167,7 @@
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -4186,7 +4192,7 @@
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -4212,7 +4218,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -4224,7 +4230,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>241</v>
       </c>
@@ -4232,7 +4238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>242</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -4257,7 +4263,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>151</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>245</v>
       </c>
@@ -4285,7 +4291,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>255</v>
       </c>
@@ -4296,7 +4302,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>258</v>
       </c>
@@ -4314,7 +4320,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>260</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>248</v>
       </c>
@@ -4336,7 +4342,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>262</v>
       </c>
@@ -4344,7 +4350,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>263</v>
       </c>
@@ -4352,7 +4358,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -4398,7 +4404,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -4407,7 +4413,7 @@
     <col min="34" max="34" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30">
+    <row r="1" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4514,7 +4520,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -4557,7 +4563,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -4572,7 +4578,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4589,7 +4595,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -4603,7 +4609,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -4623,7 +4629,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -4634,7 +4640,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="105">
+    <row r="9" spans="1:35" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>78</v>
       </c>
@@ -4672,12 +4678,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4700,7 +4706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -4724,7 +4730,7 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -4740,7 +4746,7 @@
     <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4811,7 +4817,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="12.75" customHeight="1">
+    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4836,7 +4842,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -4845,7 +4851,7 @@
       </c>
       <c r="W3" s="5"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -4862,7 +4868,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -4870,7 +4876,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -4899,7 +4905,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -4928,7 +4934,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -4942,7 +4948,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -4956,10 +4962,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V12" s="9"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="U15" s="9"/>
     </row>
   </sheetData>
@@ -4983,7 +4989,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
@@ -4992,7 +4998,7 @@
     <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -5109,7 +5115,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -5156,7 +5162,7 @@
       </c>
       <c r="W3" s="9"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -5208,7 +5214,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -5232,7 +5238,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5249,7 +5255,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -5282,7 +5288,7 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -5300,7 +5306,7 @@
     <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5371,7 +5377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -5409,7 +5415,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -5437,7 +5443,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -5451,7 +5457,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -5474,7 +5480,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -5502,7 +5508,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -5513,7 +5519,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -5545,7 +5551,7 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
@@ -5556,7 +5562,7 @@
     <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5582,7 +5588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -5596,12 +5602,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -5612,7 +5618,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -5627,7 +5633,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H9" s="9"/>
     </row>
   </sheetData>
@@ -5649,9 +5655,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5711,7 +5717,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -5733,7 +5739,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -5743,7 +5749,7 @@
       <c r="R3" s="5"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -5762,7 +5768,7 @@
       <c r="R4" s="5"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -5785,7 +5791,7 @@
       <c r="P5" s="4"/>
       <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5799,7 +5805,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>151</v>
       </c>

</xml_diff>

<commit_message>
Sweden and Geo-location method Updated for Osprey
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreySweden.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreySweden.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{ED4B3FAD-0B82-46FF-A4F9-9066E4D0E105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{587A46F4-7EC3-4E14-AA69-66442ADD8838}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{ED4B3FAD-0B82-46FF-A4F9-9066E4D0E105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0EBA668-1B94-4F2D-94DC-84FFFE7CB453}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="273">
   <si>
     <t>DataSet</t>
   </si>
@@ -892,6 +892,18 @@
   </si>
   <si>
     <t>testersemail.278@gmail.com</t>
+  </si>
+  <si>
+    <t>Product&lt;50</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Kr</t>
   </si>
 </sst>
 </file>
@@ -3306,7 +3318,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEDE721-2994-4A91-8C89-FADAE76105D8}">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -3479,7 +3491,7 @@
         <v>90</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>162</v>
+        <v>272</v>
       </c>
       <c r="T3" t="s">
         <v>91</v>
@@ -3855,7 +3867,7 @@
         <v>245</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>162</v>
+        <v>272</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>246</v>
@@ -3873,6 +3885,14 @@
       </c>
       <c r="AE23" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>269</v>
+      </c>
+      <c r="T24" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -4432,10 +4452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6E5005-1842-4D3B-9DB5-D7120C934727}">
-  <dimension ref="A1:AI9"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4443,11 +4463,11 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.7109375" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4479,82 +4499,85 @@
         <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AH1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -4575,15 +4598,18 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="O2" s="5"/>
+      <c r="K2" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="P2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="7"/>
-      <c r="AD2" t="s">
+      <c r="Q2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="7"/>
+      <c r="AE2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -4594,10 +4620,10 @@
         <v>63</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="S3" s="5"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -4606,13 +4632,13 @@
       <c r="H4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="7"/>
-      <c r="AF4" t="s">
+      <c r="S4" s="5"/>
+      <c r="T4" s="7"/>
+      <c r="AG4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4622,14 +4648,14 @@
       <c r="H5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="4"/>
-      <c r="V5" s="5"/>
-      <c r="AF5" t="s">
+      <c r="P5" s="3"/>
+      <c r="Q5" s="4"/>
+      <c r="W5" s="5"/>
+      <c r="AG5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -4639,11 +4665,11 @@
       <c r="H6" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
@@ -4663,7 +4689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -4674,17 +4700,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="AG9" s="13" t="s">
+      <c r="AH9" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="AH9" s="13" t="s">
+      <c r="AI9" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="AI9" s="16" t="s">
+      <c r="AJ9" s="16" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel changes for ospreu Sweden
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_EMEA/GoldOspreySweden.xlsx
+++ b/src/test/resources/TestData/Osprey_EMEA/GoldOspreySweden.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{ED4B3FAD-0B82-46FF-A4F9-9066E4D0E105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0EBA668-1B94-4F2D-94DC-84FFFE7CB453}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A52CE24-84AD-47B3-8E57-CA8E895D9533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="274">
   <si>
     <t>DataSet</t>
   </si>
@@ -888,12 +888,6 @@
     <t>RADIAL 34</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>testersemail.278@gmail.com</t>
-  </si>
-  <si>
     <t>Product&lt;50</t>
   </si>
   <si>
@@ -904,6 +898,15 @@
   </si>
   <si>
     <t>Kr</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>abogi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Abcd@123</t>
   </si>
 </sst>
 </file>
@@ -1077,10 +1080,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3321,7 +3320,7 @@
   <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3442,22 +3441,22 @@
         <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>272</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>272</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>273</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>63</v>
+        <v>273</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -3491,7 +3490,7 @@
         <v>90</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T3" t="s">
         <v>91</v>
@@ -3513,8 +3512,8 @@
       <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="Y4" t="s">
-        <v>267</v>
+      <c r="Y4" s="5" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -3867,7 +3866,7 @@
         <v>245</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>246</v>
@@ -3889,7 +3888,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="T24" t="s">
         <v>266</v>
@@ -3897,10 +3896,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="testersemail.278@gmail.com" xr:uid="{C94C20D5-4494-4663-8D15-E3F04F8BA838}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C94C20D5-4494-4663-8D15-E3F04F8BA838}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{0F1A9542-CB17-4A46-B151-3CB4195FE686}"/>
     <hyperlink ref="G2" r:id="rId3" xr:uid="{3D6B96F7-7492-4831-BA08-1EC319F3C995}"/>
-    <hyperlink ref="C2" r:id="rId4" display="testersemail.278@gmail.com" xr:uid="{FF5CC51C-5AD9-4693-981E-E7B0E9E657C5}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{FF5CC51C-5AD9-4693-981E-E7B0E9E657C5}"/>
     <hyperlink ref="F9" r:id="rId5" xr:uid="{D61594FB-34B8-48FF-8601-E5E62BE99A50}"/>
     <hyperlink ref="C10" r:id="rId6" xr:uid="{5D1A5D25-CA74-4312-B274-A09F60758C65}"/>
     <hyperlink ref="C12" r:id="rId7" xr:uid="{05504D73-D67C-47D1-B503-0C5ECD72787A}"/>
@@ -3911,7 +3910,7 @@
     <hyperlink ref="B16" r:id="rId12" xr:uid="{4F884725-7BD6-4040-9EB4-E29F2ED09129}"/>
     <hyperlink ref="C16" r:id="rId13" xr:uid="{50B14846-390B-41D6-AC9B-F1AB298F8D8C}"/>
     <hyperlink ref="D2" r:id="rId14" xr:uid="{EB2A1C32-0843-4A07-853D-B23E75EE8B0C}"/>
-    <hyperlink ref="E2" r:id="rId15" xr:uid="{3C78F6C6-2B5D-49D9-9AE0-669EF34B6FF5}"/>
+    <hyperlink ref="E2" r:id="rId15" xr:uid="{B117E320-3F42-47BF-BEB2-29D11DBB11E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>
@@ -4499,7 +4498,7 @@
         <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>39</v>
@@ -4599,7 +4598,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>

</xml_diff>